<commit_message>
Add LVDS_25 IOSTANDARD back
</commit_message>
<xml_diff>
--- a/pins.xlsx
+++ b/pins.xlsx
@@ -1855,7 +1855,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>DS_SDO[1]</t>
+          <t>DS_SDO[0]</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>DS_SCLK[1]</t>
+          <t>DS_SCLK[0]</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1915,7 +1915,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>DS_CSB[1]</t>
+          <t>DS_CSB[0]</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1959,7 +1959,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>DS_SDI[1]</t>
+          <t>DS_SDI[0]</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>DS_SDO[2]</t>
+          <t>DS_SDO[1]</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2019,7 +2019,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>DS_SCLK[2]</t>
+          <t>DS_SCLK[1]</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>DS_CSB[2]</t>
+          <t>DS_CSB[1]</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2079,7 +2079,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>DS_SDI[2]</t>
+          <t>DS_SDI[1]</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>EN_IPUMP[1]</t>
+          <t>EN_IPUMP[0]</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2497,7 +2497,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>EN_IPUMP[2]</t>
+          <t>EN_IPUMP[1]</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -2698,7 +2698,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -2728,7 +2728,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -2758,7 +2758,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -2878,7 +2878,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -2938,7 +2938,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -2982,7 +2982,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3042,7 +3042,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3072,7 +3072,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3132,7 +3132,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3162,7 +3162,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3222,7 +3222,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3266,7 +3266,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3326,7 +3326,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3356,7 +3356,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3546,7 +3546,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3720,7 +3720,7 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3750,7 +3750,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3780,7 +3780,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3810,7 +3810,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3840,7 +3840,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3870,7 +3870,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3900,7 +3900,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3930,7 +3930,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3960,7 +3960,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -3990,7 +3990,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -4034,7 +4034,7 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -4064,7 +4064,7 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -4090,7 +4090,7 @@
       <c r="E142" t="inlineStr"/>
       <c r="F142" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -4120,7 +4120,7 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>LVCMOS25</t>
+          <t>LVDS_25</t>
         </is>
       </c>
     </row>
@@ -4239,7 +4239,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>A_EN_HV[1]</t>
+          <t>A_EN_HV[0]</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4279,7 +4279,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>A_EN_HV[2]</t>
+          <t>A_EN_HV[1]</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -4305,7 +4305,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>A_EN_HV[3]</t>
+          <t>A_EN_HV[2]</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">

</xml_diff>